<commit_message>
translated the iPython notebook to english and added some more content changed input files to english
</commit_message>
<xml_diff>
--- a/EBC-Python-101/Messung2.xlsx
+++ b/EBC-Python-101/Messung2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\ebc-python_library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\EBC-Tutorials\EBC-Python-101\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,10 +21,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Ventilstellung</t>
+    <t>travel</t>
   </si>
   <si>
-    <t>Heizleistung</t>
+    <t>heating power</t>
   </si>
 </sst>
 </file>
@@ -833,7 +833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>